<commit_message>
fix the damn fob mode pls for apply cell to be working
</commit_message>
<xml_diff>
--- a/TEMPLATE/MOTO.xlsx
+++ b/TEMPLATE/MOTO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\gen_inv\TEMPLATE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\refactor code\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9007C2E9-21E8-4096-ACFF-61D4442530C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8A1599-A192-4780-A26A-D7322EA68FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="1" r:id="rId1"/>
@@ -18,8 +18,8 @@
     <sheet name="Packing list" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$1:$G$32</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Contract!$A$1:$G$29</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Invoice!$A$1:$G$28</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Packing list'!$A$1:$I$32</definedName>
   </definedNames>
   <calcPr calcId="191029" fullPrecision="0"/>
@@ -909,6 +909,18 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -927,28 +939,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -972,285 +972,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>315595</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1549400</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>130811</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="微信图片_20230906130651">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10671175" y="14919960"/>
-          <a:ext cx="3435350" cy="1896745"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>1734820</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>217170</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>53975</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>323849</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2" descr="微信图片_20230906130654">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12377420" y="14087475"/>
-          <a:ext cx="2148205" cy="1207770"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>400050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>233680</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>188595</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 2" descr="微信图片_20230906130654">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13230225" y="14373225"/>
-          <a:ext cx="2148205" cy="1207770"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>425450</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>296545</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 1" descr="微信图片_20230906130651">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13087350" y="13792200"/>
-          <a:ext cx="3435350" cy="1896745"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>649344</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>268643</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>739065</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>737198</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="图片 1" descr="微信图片_20230906130651">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="14253285" y="18287702"/>
-          <a:ext cx="3440280" cy="1902908"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>403935</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>546175</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>871743</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>327996</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="图片 2" descr="微信图片_20230906130654">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="15677553" y="19999587"/>
-          <a:ext cx="2148690" cy="1204968"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1511,10 +1232,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:XFD87"/>
+  <dimension ref="A1:XFD79"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="15"/>
@@ -1916,7 +1637,7 @@
       <c r="M32" s="60"/>
       <c r="XFD32" s="60"/>
     </row>
-    <row r="33" spans="1:13 16384:16384" s="55" customFormat="1" ht="39">
+    <row r="33" spans="1:45 16384:16384" s="55" customFormat="1" ht="39">
       <c r="A33" s="60"/>
       <c r="B33" s="60"/>
       <c r="C33" s="60"/>
@@ -1930,9 +1651,41 @@
       <c r="K33" s="60"/>
       <c r="L33" s="60"/>
       <c r="M33" s="60"/>
+      <c r="N33" s="60"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="60"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="60"/>
+      <c r="T33" s="60"/>
+      <c r="U33" s="60"/>
+      <c r="V33" s="60"/>
+      <c r="W33" s="60"/>
+      <c r="X33" s="60"/>
+      <c r="Y33" s="60"/>
+      <c r="Z33" s="60"/>
+      <c r="AA33" s="60"/>
+      <c r="AB33" s="60"/>
+      <c r="AC33" s="60"/>
+      <c r="AD33" s="60"/>
+      <c r="AE33" s="60"/>
+      <c r="AF33" s="60"/>
+      <c r="AG33" s="60"/>
+      <c r="AH33" s="60"/>
+      <c r="AI33" s="60"/>
+      <c r="AJ33" s="60"/>
+      <c r="AK33" s="60"/>
+      <c r="AL33" s="60"/>
+      <c r="AM33" s="60"/>
+      <c r="AN33" s="60"/>
+      <c r="AO33" s="60"/>
+      <c r="AP33" s="60"/>
+      <c r="AQ33" s="60"/>
+      <c r="AR33" s="60"/>
+      <c r="AS33" s="60"/>
       <c r="XFD33" s="60"/>
     </row>
-    <row r="34" spans="1:13 16384:16384" s="55" customFormat="1" ht="39">
+    <row r="34" spans="1:45 16384:16384" s="55" customFormat="1" ht="39">
       <c r="A34" s="60"/>
       <c r="B34" s="60"/>
       <c r="C34" s="60"/>
@@ -1946,9 +1699,41 @@
       <c r="K34" s="60"/>
       <c r="L34" s="60"/>
       <c r="M34" s="60"/>
+      <c r="N34" s="60"/>
+      <c r="O34" s="60"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="60"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="60"/>
+      <c r="T34" s="60"/>
+      <c r="U34" s="60"/>
+      <c r="V34" s="60"/>
+      <c r="W34" s="60"/>
+      <c r="X34" s="60"/>
+      <c r="Y34" s="60"/>
+      <c r="Z34" s="60"/>
+      <c r="AA34" s="60"/>
+      <c r="AB34" s="60"/>
+      <c r="AC34" s="60"/>
+      <c r="AD34" s="60"/>
+      <c r="AE34" s="60"/>
+      <c r="AF34" s="60"/>
+      <c r="AG34" s="60"/>
+      <c r="AH34" s="60"/>
+      <c r="AI34" s="60"/>
+      <c r="AJ34" s="60"/>
+      <c r="AK34" s="60"/>
+      <c r="AL34" s="60"/>
+      <c r="AM34" s="60"/>
+      <c r="AN34" s="60"/>
+      <c r="AO34" s="60"/>
+      <c r="AP34" s="60"/>
+      <c r="AQ34" s="60"/>
+      <c r="AR34" s="60"/>
+      <c r="AS34" s="60"/>
       <c r="XFD34" s="60"/>
     </row>
-    <row r="35" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="35" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A35" s="60"/>
       <c r="B35" s="60"/>
       <c r="C35" s="60"/>
@@ -1962,9 +1747,41 @@
       <c r="K35" s="60"/>
       <c r="L35" s="60"/>
       <c r="M35" s="60"/>
+      <c r="N35" s="60"/>
+      <c r="O35" s="60"/>
+      <c r="P35" s="60"/>
+      <c r="Q35" s="60"/>
+      <c r="R35" s="60"/>
+      <c r="S35" s="60"/>
+      <c r="T35" s="60"/>
+      <c r="U35" s="60"/>
+      <c r="V35" s="60"/>
+      <c r="W35" s="60"/>
+      <c r="X35" s="60"/>
+      <c r="Y35" s="60"/>
+      <c r="Z35" s="60"/>
+      <c r="AA35" s="60"/>
+      <c r="AB35" s="60"/>
+      <c r="AC35" s="60"/>
+      <c r="AD35" s="60"/>
+      <c r="AE35" s="60"/>
+      <c r="AF35" s="60"/>
+      <c r="AG35" s="60"/>
+      <c r="AH35" s="60"/>
+      <c r="AI35" s="60"/>
+      <c r="AJ35" s="60"/>
+      <c r="AK35" s="60"/>
+      <c r="AL35" s="60"/>
+      <c r="AM35" s="60"/>
+      <c r="AN35" s="60"/>
+      <c r="AO35" s="60"/>
+      <c r="AP35" s="60"/>
+      <c r="AQ35" s="60"/>
+      <c r="AR35" s="60"/>
+      <c r="AS35" s="60"/>
       <c r="XFD35" s="60"/>
     </row>
-    <row r="36" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="36" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A36" s="60"/>
       <c r="B36" s="60"/>
       <c r="C36" s="60"/>
@@ -1978,9 +1795,41 @@
       <c r="K36" s="60"/>
       <c r="L36" s="60"/>
       <c r="M36" s="60"/>
+      <c r="N36" s="60"/>
+      <c r="O36" s="60"/>
+      <c r="P36" s="60"/>
+      <c r="Q36" s="60"/>
+      <c r="R36" s="60"/>
+      <c r="S36" s="60"/>
+      <c r="T36" s="60"/>
+      <c r="U36" s="60"/>
+      <c r="V36" s="60"/>
+      <c r="W36" s="60"/>
+      <c r="X36" s="60"/>
+      <c r="Y36" s="60"/>
+      <c r="Z36" s="60"/>
+      <c r="AA36" s="60"/>
+      <c r="AB36" s="60"/>
+      <c r="AC36" s="60"/>
+      <c r="AD36" s="60"/>
+      <c r="AE36" s="60"/>
+      <c r="AF36" s="60"/>
+      <c r="AG36" s="60"/>
+      <c r="AH36" s="60"/>
+      <c r="AI36" s="60"/>
+      <c r="AJ36" s="60"/>
+      <c r="AK36" s="60"/>
+      <c r="AL36" s="60"/>
+      <c r="AM36" s="60"/>
+      <c r="AN36" s="60"/>
+      <c r="AO36" s="60"/>
+      <c r="AP36" s="60"/>
+      <c r="AQ36" s="60"/>
+      <c r="AR36" s="60"/>
+      <c r="AS36" s="60"/>
       <c r="XFD36" s="60"/>
     </row>
-    <row r="37" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="37" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A37" s="60"/>
       <c r="B37" s="60"/>
       <c r="C37" s="60"/>
@@ -1994,9 +1843,41 @@
       <c r="K37" s="60"/>
       <c r="L37" s="60"/>
       <c r="M37" s="60"/>
+      <c r="N37" s="60"/>
+      <c r="O37" s="60"/>
+      <c r="P37" s="60"/>
+      <c r="Q37" s="60"/>
+      <c r="R37" s="60"/>
+      <c r="S37" s="60"/>
+      <c r="T37" s="60"/>
+      <c r="U37" s="60"/>
+      <c r="V37" s="60"/>
+      <c r="W37" s="60"/>
+      <c r="X37" s="60"/>
+      <c r="Y37" s="60"/>
+      <c r="Z37" s="60"/>
+      <c r="AA37" s="60"/>
+      <c r="AB37" s="60"/>
+      <c r="AC37" s="60"/>
+      <c r="AD37" s="60"/>
+      <c r="AE37" s="60"/>
+      <c r="AF37" s="60"/>
+      <c r="AG37" s="60"/>
+      <c r="AH37" s="60"/>
+      <c r="AI37" s="60"/>
+      <c r="AJ37" s="60"/>
+      <c r="AK37" s="60"/>
+      <c r="AL37" s="60"/>
+      <c r="AM37" s="60"/>
+      <c r="AN37" s="60"/>
+      <c r="AO37" s="60"/>
+      <c r="AP37" s="60"/>
+      <c r="AQ37" s="60"/>
+      <c r="AR37" s="60"/>
+      <c r="AS37" s="60"/>
       <c r="XFD37" s="60"/>
     </row>
-    <row r="38" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="38" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A38" s="60"/>
       <c r="B38" s="60"/>
       <c r="C38" s="60"/>
@@ -2010,9 +1891,41 @@
       <c r="K38" s="60"/>
       <c r="L38" s="60"/>
       <c r="M38" s="60"/>
+      <c r="N38" s="60"/>
+      <c r="O38" s="60"/>
+      <c r="P38" s="60"/>
+      <c r="Q38" s="60"/>
+      <c r="R38" s="60"/>
+      <c r="S38" s="60"/>
+      <c r="T38" s="60"/>
+      <c r="U38" s="60"/>
+      <c r="V38" s="60"/>
+      <c r="W38" s="60"/>
+      <c r="X38" s="60"/>
+      <c r="Y38" s="60"/>
+      <c r="Z38" s="60"/>
+      <c r="AA38" s="60"/>
+      <c r="AB38" s="60"/>
+      <c r="AC38" s="60"/>
+      <c r="AD38" s="60"/>
+      <c r="AE38" s="60"/>
+      <c r="AF38" s="60"/>
+      <c r="AG38" s="60"/>
+      <c r="AH38" s="60"/>
+      <c r="AI38" s="60"/>
+      <c r="AJ38" s="60"/>
+      <c r="AK38" s="60"/>
+      <c r="AL38" s="60"/>
+      <c r="AM38" s="60"/>
+      <c r="AN38" s="60"/>
+      <c r="AO38" s="60"/>
+      <c r="AP38" s="60"/>
+      <c r="AQ38" s="60"/>
+      <c r="AR38" s="60"/>
+      <c r="AS38" s="60"/>
       <c r="XFD38" s="60"/>
     </row>
-    <row r="39" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="39" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A39" s="60"/>
       <c r="B39" s="60"/>
       <c r="C39" s="60"/>
@@ -2026,9 +1939,41 @@
       <c r="K39" s="60"/>
       <c r="L39" s="60"/>
       <c r="M39" s="60"/>
+      <c r="N39" s="60"/>
+      <c r="O39" s="60"/>
+      <c r="P39" s="60"/>
+      <c r="Q39" s="60"/>
+      <c r="R39" s="60"/>
+      <c r="S39" s="60"/>
+      <c r="T39" s="60"/>
+      <c r="U39" s="60"/>
+      <c r="V39" s="60"/>
+      <c r="W39" s="60"/>
+      <c r="X39" s="60"/>
+      <c r="Y39" s="60"/>
+      <c r="Z39" s="60"/>
+      <c r="AA39" s="60"/>
+      <c r="AB39" s="60"/>
+      <c r="AC39" s="60"/>
+      <c r="AD39" s="60"/>
+      <c r="AE39" s="60"/>
+      <c r="AF39" s="60"/>
+      <c r="AG39" s="60"/>
+      <c r="AH39" s="60"/>
+      <c r="AI39" s="60"/>
+      <c r="AJ39" s="60"/>
+      <c r="AK39" s="60"/>
+      <c r="AL39" s="60"/>
+      <c r="AM39" s="60"/>
+      <c r="AN39" s="60"/>
+      <c r="AO39" s="60"/>
+      <c r="AP39" s="60"/>
+      <c r="AQ39" s="60"/>
+      <c r="AR39" s="60"/>
+      <c r="AS39" s="60"/>
       <c r="XFD39" s="60"/>
     </row>
-    <row r="40" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="40" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A40" s="60"/>
       <c r="B40" s="60"/>
       <c r="C40" s="60"/>
@@ -2042,9 +1987,41 @@
       <c r="K40" s="60"/>
       <c r="L40" s="60"/>
       <c r="M40" s="60"/>
+      <c r="N40" s="60"/>
+      <c r="O40" s="60"/>
+      <c r="P40" s="60"/>
+      <c r="Q40" s="60"/>
+      <c r="R40" s="60"/>
+      <c r="S40" s="60"/>
+      <c r="T40" s="60"/>
+      <c r="U40" s="60"/>
+      <c r="V40" s="60"/>
+      <c r="W40" s="60"/>
+      <c r="X40" s="60"/>
+      <c r="Y40" s="60"/>
+      <c r="Z40" s="60"/>
+      <c r="AA40" s="60"/>
+      <c r="AB40" s="60"/>
+      <c r="AC40" s="60"/>
+      <c r="AD40" s="60"/>
+      <c r="AE40" s="60"/>
+      <c r="AF40" s="60"/>
+      <c r="AG40" s="60"/>
+      <c r="AH40" s="60"/>
+      <c r="AI40" s="60"/>
+      <c r="AJ40" s="60"/>
+      <c r="AK40" s="60"/>
+      <c r="AL40" s="60"/>
+      <c r="AM40" s="60"/>
+      <c r="AN40" s="60"/>
+      <c r="AO40" s="60"/>
+      <c r="AP40" s="60"/>
+      <c r="AQ40" s="60"/>
+      <c r="AR40" s="60"/>
+      <c r="AS40" s="60"/>
       <c r="XFD40" s="60"/>
     </row>
-    <row r="41" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="41" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A41" s="60"/>
       <c r="B41" s="60"/>
       <c r="C41" s="60"/>
@@ -2058,9 +2035,41 @@
       <c r="K41" s="60"/>
       <c r="L41" s="60"/>
       <c r="M41" s="60"/>
+      <c r="N41" s="60"/>
+      <c r="O41" s="60"/>
+      <c r="P41" s="60"/>
+      <c r="Q41" s="60"/>
+      <c r="R41" s="60"/>
+      <c r="S41" s="60"/>
+      <c r="T41" s="60"/>
+      <c r="U41" s="60"/>
+      <c r="V41" s="60"/>
+      <c r="W41" s="60"/>
+      <c r="X41" s="60"/>
+      <c r="Y41" s="60"/>
+      <c r="Z41" s="60"/>
+      <c r="AA41" s="60"/>
+      <c r="AB41" s="60"/>
+      <c r="AC41" s="60"/>
+      <c r="AD41" s="60"/>
+      <c r="AE41" s="60"/>
+      <c r="AF41" s="60"/>
+      <c r="AG41" s="60"/>
+      <c r="AH41" s="60"/>
+      <c r="AI41" s="60"/>
+      <c r="AJ41" s="60"/>
+      <c r="AK41" s="60"/>
+      <c r="AL41" s="60"/>
+      <c r="AM41" s="60"/>
+      <c r="AN41" s="60"/>
+      <c r="AO41" s="60"/>
+      <c r="AP41" s="60"/>
+      <c r="AQ41" s="60"/>
+      <c r="AR41" s="60"/>
+      <c r="AS41" s="60"/>
       <c r="XFD41" s="60"/>
     </row>
-    <row r="42" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="42" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A42" s="60"/>
       <c r="B42" s="60"/>
       <c r="C42" s="60"/>
@@ -2074,9 +2083,41 @@
       <c r="K42" s="60"/>
       <c r="L42" s="60"/>
       <c r="M42" s="60"/>
+      <c r="N42" s="60"/>
+      <c r="O42" s="60"/>
+      <c r="P42" s="60"/>
+      <c r="Q42" s="60"/>
+      <c r="R42" s="60"/>
+      <c r="S42" s="60"/>
+      <c r="T42" s="60"/>
+      <c r="U42" s="60"/>
+      <c r="V42" s="60"/>
+      <c r="W42" s="60"/>
+      <c r="X42" s="60"/>
+      <c r="Y42" s="60"/>
+      <c r="Z42" s="60"/>
+      <c r="AA42" s="60"/>
+      <c r="AB42" s="60"/>
+      <c r="AC42" s="60"/>
+      <c r="AD42" s="60"/>
+      <c r="AE42" s="60"/>
+      <c r="AF42" s="60"/>
+      <c r="AG42" s="60"/>
+      <c r="AH42" s="60"/>
+      <c r="AI42" s="60"/>
+      <c r="AJ42" s="60"/>
+      <c r="AK42" s="60"/>
+      <c r="AL42" s="60"/>
+      <c r="AM42" s="60"/>
+      <c r="AN42" s="60"/>
+      <c r="AO42" s="60"/>
+      <c r="AP42" s="60"/>
+      <c r="AQ42" s="60"/>
+      <c r="AR42" s="60"/>
+      <c r="AS42" s="60"/>
       <c r="XFD42" s="60"/>
     </row>
-    <row r="43" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="43" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A43" s="60"/>
       <c r="B43" s="60"/>
       <c r="C43" s="60"/>
@@ -2090,9 +2131,41 @@
       <c r="K43" s="60"/>
       <c r="L43" s="60"/>
       <c r="M43" s="60"/>
+      <c r="N43" s="60"/>
+      <c r="O43" s="60"/>
+      <c r="P43" s="60"/>
+      <c r="Q43" s="60"/>
+      <c r="R43" s="60"/>
+      <c r="S43" s="60"/>
+      <c r="T43" s="60"/>
+      <c r="U43" s="60"/>
+      <c r="V43" s="60"/>
+      <c r="W43" s="60"/>
+      <c r="X43" s="60"/>
+      <c r="Y43" s="60"/>
+      <c r="Z43" s="60"/>
+      <c r="AA43" s="60"/>
+      <c r="AB43" s="60"/>
+      <c r="AC43" s="60"/>
+      <c r="AD43" s="60"/>
+      <c r="AE43" s="60"/>
+      <c r="AF43" s="60"/>
+      <c r="AG43" s="60"/>
+      <c r="AH43" s="60"/>
+      <c r="AI43" s="60"/>
+      <c r="AJ43" s="60"/>
+      <c r="AK43" s="60"/>
+      <c r="AL43" s="60"/>
+      <c r="AM43" s="60"/>
+      <c r="AN43" s="60"/>
+      <c r="AO43" s="60"/>
+      <c r="AP43" s="60"/>
+      <c r="AQ43" s="60"/>
+      <c r="AR43" s="60"/>
+      <c r="AS43" s="60"/>
       <c r="XFD43" s="60"/>
     </row>
-    <row r="44" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="44" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A44" s="60"/>
       <c r="B44" s="60"/>
       <c r="C44" s="60"/>
@@ -2106,9 +2179,41 @@
       <c r="K44" s="60"/>
       <c r="L44" s="60"/>
       <c r="M44" s="60"/>
+      <c r="N44" s="60"/>
+      <c r="O44" s="60"/>
+      <c r="P44" s="60"/>
+      <c r="Q44" s="60"/>
+      <c r="R44" s="60"/>
+      <c r="S44" s="60"/>
+      <c r="T44" s="60"/>
+      <c r="U44" s="60"/>
+      <c r="V44" s="60"/>
+      <c r="W44" s="60"/>
+      <c r="X44" s="60"/>
+      <c r="Y44" s="60"/>
+      <c r="Z44" s="60"/>
+      <c r="AA44" s="60"/>
+      <c r="AB44" s="60"/>
+      <c r="AC44" s="60"/>
+      <c r="AD44" s="60"/>
+      <c r="AE44" s="60"/>
+      <c r="AF44" s="60"/>
+      <c r="AG44" s="60"/>
+      <c r="AH44" s="60"/>
+      <c r="AI44" s="60"/>
+      <c r="AJ44" s="60"/>
+      <c r="AK44" s="60"/>
+      <c r="AL44" s="60"/>
+      <c r="AM44" s="60"/>
+      <c r="AN44" s="60"/>
+      <c r="AO44" s="60"/>
+      <c r="AP44" s="60"/>
+      <c r="AQ44" s="60"/>
+      <c r="AR44" s="60"/>
+      <c r="AS44" s="60"/>
       <c r="XFD44" s="60"/>
     </row>
-    <row r="45" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="45" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A45" s="60"/>
       <c r="B45" s="60"/>
       <c r="C45" s="60"/>
@@ -2122,9 +2227,41 @@
       <c r="K45" s="60"/>
       <c r="L45" s="60"/>
       <c r="M45" s="60"/>
+      <c r="N45" s="60"/>
+      <c r="O45" s="60"/>
+      <c r="P45" s="60"/>
+      <c r="Q45" s="60"/>
+      <c r="R45" s="60"/>
+      <c r="S45" s="60"/>
+      <c r="T45" s="60"/>
+      <c r="U45" s="60"/>
+      <c r="V45" s="60"/>
+      <c r="W45" s="60"/>
+      <c r="X45" s="60"/>
+      <c r="Y45" s="60"/>
+      <c r="Z45" s="60"/>
+      <c r="AA45" s="60"/>
+      <c r="AB45" s="60"/>
+      <c r="AC45" s="60"/>
+      <c r="AD45" s="60"/>
+      <c r="AE45" s="60"/>
+      <c r="AF45" s="60"/>
+      <c r="AG45" s="60"/>
+      <c r="AH45" s="60"/>
+      <c r="AI45" s="60"/>
+      <c r="AJ45" s="60"/>
+      <c r="AK45" s="60"/>
+      <c r="AL45" s="60"/>
+      <c r="AM45" s="60"/>
+      <c r="AN45" s="60"/>
+      <c r="AO45" s="60"/>
+      <c r="AP45" s="60"/>
+      <c r="AQ45" s="60"/>
+      <c r="AR45" s="60"/>
+      <c r="AS45" s="60"/>
       <c r="XFD45" s="60"/>
     </row>
-    <row r="46" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="46" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A46" s="60"/>
       <c r="B46" s="60"/>
       <c r="C46" s="60"/>
@@ -2138,9 +2275,41 @@
       <c r="K46" s="60"/>
       <c r="L46" s="60"/>
       <c r="M46" s="60"/>
+      <c r="N46" s="60"/>
+      <c r="O46" s="60"/>
+      <c r="P46" s="60"/>
+      <c r="Q46" s="60"/>
+      <c r="R46" s="60"/>
+      <c r="S46" s="60"/>
+      <c r="T46" s="60"/>
+      <c r="U46" s="60"/>
+      <c r="V46" s="60"/>
+      <c r="W46" s="60"/>
+      <c r="X46" s="60"/>
+      <c r="Y46" s="60"/>
+      <c r="Z46" s="60"/>
+      <c r="AA46" s="60"/>
+      <c r="AB46" s="60"/>
+      <c r="AC46" s="60"/>
+      <c r="AD46" s="60"/>
+      <c r="AE46" s="60"/>
+      <c r="AF46" s="60"/>
+      <c r="AG46" s="60"/>
+      <c r="AH46" s="60"/>
+      <c r="AI46" s="60"/>
+      <c r="AJ46" s="60"/>
+      <c r="AK46" s="60"/>
+      <c r="AL46" s="60"/>
+      <c r="AM46" s="60"/>
+      <c r="AN46" s="60"/>
+      <c r="AO46" s="60"/>
+      <c r="AP46" s="60"/>
+      <c r="AQ46" s="60"/>
+      <c r="AR46" s="60"/>
+      <c r="AS46" s="60"/>
       <c r="XFD46" s="60"/>
     </row>
-    <row r="47" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="47" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A47" s="60"/>
       <c r="B47" s="60"/>
       <c r="C47" s="60"/>
@@ -2154,9 +2323,41 @@
       <c r="K47" s="60"/>
       <c r="L47" s="60"/>
       <c r="M47" s="60"/>
+      <c r="N47" s="60"/>
+      <c r="O47" s="60"/>
+      <c r="P47" s="60"/>
+      <c r="Q47" s="60"/>
+      <c r="R47" s="60"/>
+      <c r="S47" s="60"/>
+      <c r="T47" s="60"/>
+      <c r="U47" s="60"/>
+      <c r="V47" s="60"/>
+      <c r="W47" s="60"/>
+      <c r="X47" s="60"/>
+      <c r="Y47" s="60"/>
+      <c r="Z47" s="60"/>
+      <c r="AA47" s="60"/>
+      <c r="AB47" s="60"/>
+      <c r="AC47" s="60"/>
+      <c r="AD47" s="60"/>
+      <c r="AE47" s="60"/>
+      <c r="AF47" s="60"/>
+      <c r="AG47" s="60"/>
+      <c r="AH47" s="60"/>
+      <c r="AI47" s="60"/>
+      <c r="AJ47" s="60"/>
+      <c r="AK47" s="60"/>
+      <c r="AL47" s="60"/>
+      <c r="AM47" s="60"/>
+      <c r="AN47" s="60"/>
+      <c r="AO47" s="60"/>
+      <c r="AP47" s="60"/>
+      <c r="AQ47" s="60"/>
+      <c r="AR47" s="60"/>
+      <c r="AS47" s="60"/>
       <c r="XFD47" s="60"/>
     </row>
-    <row r="48" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="48" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A48" s="60"/>
       <c r="B48" s="60"/>
       <c r="C48" s="60"/>
@@ -2170,9 +2371,41 @@
       <c r="K48" s="60"/>
       <c r="L48" s="60"/>
       <c r="M48" s="60"/>
+      <c r="N48" s="60"/>
+      <c r="O48" s="60"/>
+      <c r="P48" s="60"/>
+      <c r="Q48" s="60"/>
+      <c r="R48" s="60"/>
+      <c r="S48" s="60"/>
+      <c r="T48" s="60"/>
+      <c r="U48" s="60"/>
+      <c r="V48" s="60"/>
+      <c r="W48" s="60"/>
+      <c r="X48" s="60"/>
+      <c r="Y48" s="60"/>
+      <c r="Z48" s="60"/>
+      <c r="AA48" s="60"/>
+      <c r="AB48" s="60"/>
+      <c r="AC48" s="60"/>
+      <c r="AD48" s="60"/>
+      <c r="AE48" s="60"/>
+      <c r="AF48" s="60"/>
+      <c r="AG48" s="60"/>
+      <c r="AH48" s="60"/>
+      <c r="AI48" s="60"/>
+      <c r="AJ48" s="60"/>
+      <c r="AK48" s="60"/>
+      <c r="AL48" s="60"/>
+      <c r="AM48" s="60"/>
+      <c r="AN48" s="60"/>
+      <c r="AO48" s="60"/>
+      <c r="AP48" s="60"/>
+      <c r="AQ48" s="60"/>
+      <c r="AR48" s="60"/>
+      <c r="AS48" s="60"/>
       <c r="XFD48" s="60"/>
     </row>
-    <row r="49" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="49" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A49" s="60"/>
       <c r="B49" s="60"/>
       <c r="C49" s="60"/>
@@ -2186,9 +2419,41 @@
       <c r="K49" s="60"/>
       <c r="L49" s="60"/>
       <c r="M49" s="60"/>
+      <c r="N49" s="60"/>
+      <c r="O49" s="60"/>
+      <c r="P49" s="60"/>
+      <c r="Q49" s="60"/>
+      <c r="R49" s="60"/>
+      <c r="S49" s="60"/>
+      <c r="T49" s="60"/>
+      <c r="U49" s="60"/>
+      <c r="V49" s="60"/>
+      <c r="W49" s="60"/>
+      <c r="X49" s="60"/>
+      <c r="Y49" s="60"/>
+      <c r="Z49" s="60"/>
+      <c r="AA49" s="60"/>
+      <c r="AB49" s="60"/>
+      <c r="AC49" s="60"/>
+      <c r="AD49" s="60"/>
+      <c r="AE49" s="60"/>
+      <c r="AF49" s="60"/>
+      <c r="AG49" s="60"/>
+      <c r="AH49" s="60"/>
+      <c r="AI49" s="60"/>
+      <c r="AJ49" s="60"/>
+      <c r="AK49" s="60"/>
+      <c r="AL49" s="60"/>
+      <c r="AM49" s="60"/>
+      <c r="AN49" s="60"/>
+      <c r="AO49" s="60"/>
+      <c r="AP49" s="60"/>
+      <c r="AQ49" s="60"/>
+      <c r="AR49" s="60"/>
+      <c r="AS49" s="60"/>
       <c r="XFD49" s="60"/>
     </row>
-    <row r="50" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="50" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A50" s="60"/>
       <c r="B50" s="60"/>
       <c r="C50" s="60"/>
@@ -2202,9 +2467,41 @@
       <c r="K50" s="60"/>
       <c r="L50" s="60"/>
       <c r="M50" s="60"/>
+      <c r="N50" s="60"/>
+      <c r="O50" s="60"/>
+      <c r="P50" s="60"/>
+      <c r="Q50" s="60"/>
+      <c r="R50" s="60"/>
+      <c r="S50" s="60"/>
+      <c r="T50" s="60"/>
+      <c r="U50" s="60"/>
+      <c r="V50" s="60"/>
+      <c r="W50" s="60"/>
+      <c r="X50" s="60"/>
+      <c r="Y50" s="60"/>
+      <c r="Z50" s="60"/>
+      <c r="AA50" s="60"/>
+      <c r="AB50" s="60"/>
+      <c r="AC50" s="60"/>
+      <c r="AD50" s="60"/>
+      <c r="AE50" s="60"/>
+      <c r="AF50" s="60"/>
+      <c r="AG50" s="60"/>
+      <c r="AH50" s="60"/>
+      <c r="AI50" s="60"/>
+      <c r="AJ50" s="60"/>
+      <c r="AK50" s="60"/>
+      <c r="AL50" s="60"/>
+      <c r="AM50" s="60"/>
+      <c r="AN50" s="60"/>
+      <c r="AO50" s="60"/>
+      <c r="AP50" s="60"/>
+      <c r="AQ50" s="60"/>
+      <c r="AR50" s="60"/>
+      <c r="AS50" s="60"/>
       <c r="XFD50" s="60"/>
     </row>
-    <row r="51" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="51" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A51" s="60"/>
       <c r="B51" s="60"/>
       <c r="C51" s="60"/>
@@ -2218,9 +2515,41 @@
       <c r="K51" s="60"/>
       <c r="L51" s="60"/>
       <c r="M51" s="60"/>
+      <c r="N51" s="60"/>
+      <c r="O51" s="60"/>
+      <c r="P51" s="60"/>
+      <c r="Q51" s="60"/>
+      <c r="R51" s="60"/>
+      <c r="S51" s="60"/>
+      <c r="T51" s="60"/>
+      <c r="U51" s="60"/>
+      <c r="V51" s="60"/>
+      <c r="W51" s="60"/>
+      <c r="X51" s="60"/>
+      <c r="Y51" s="60"/>
+      <c r="Z51" s="60"/>
+      <c r="AA51" s="60"/>
+      <c r="AB51" s="60"/>
+      <c r="AC51" s="60"/>
+      <c r="AD51" s="60"/>
+      <c r="AE51" s="60"/>
+      <c r="AF51" s="60"/>
+      <c r="AG51" s="60"/>
+      <c r="AH51" s="60"/>
+      <c r="AI51" s="60"/>
+      <c r="AJ51" s="60"/>
+      <c r="AK51" s="60"/>
+      <c r="AL51" s="60"/>
+      <c r="AM51" s="60"/>
+      <c r="AN51" s="60"/>
+      <c r="AO51" s="60"/>
+      <c r="AP51" s="60"/>
+      <c r="AQ51" s="60"/>
+      <c r="AR51" s="60"/>
+      <c r="AS51" s="60"/>
       <c r="XFD51" s="60"/>
     </row>
-    <row r="52" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="52" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A52" s="60"/>
       <c r="B52" s="60"/>
       <c r="C52" s="60"/>
@@ -2234,9 +2563,41 @@
       <c r="K52" s="60"/>
       <c r="L52" s="60"/>
       <c r="M52" s="60"/>
+      <c r="N52" s="60"/>
+      <c r="O52" s="60"/>
+      <c r="P52" s="60"/>
+      <c r="Q52" s="60"/>
+      <c r="R52" s="60"/>
+      <c r="S52" s="60"/>
+      <c r="T52" s="60"/>
+      <c r="U52" s="60"/>
+      <c r="V52" s="60"/>
+      <c r="W52" s="60"/>
+      <c r="X52" s="60"/>
+      <c r="Y52" s="60"/>
+      <c r="Z52" s="60"/>
+      <c r="AA52" s="60"/>
+      <c r="AB52" s="60"/>
+      <c r="AC52" s="60"/>
+      <c r="AD52" s="60"/>
+      <c r="AE52" s="60"/>
+      <c r="AF52" s="60"/>
+      <c r="AG52" s="60"/>
+      <c r="AH52" s="60"/>
+      <c r="AI52" s="60"/>
+      <c r="AJ52" s="60"/>
+      <c r="AK52" s="60"/>
+      <c r="AL52" s="60"/>
+      <c r="AM52" s="60"/>
+      <c r="AN52" s="60"/>
+      <c r="AO52" s="60"/>
+      <c r="AP52" s="60"/>
+      <c r="AQ52" s="60"/>
+      <c r="AR52" s="60"/>
+      <c r="AS52" s="60"/>
       <c r="XFD52" s="60"/>
     </row>
-    <row r="53" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="53" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A53" s="60"/>
       <c r="B53" s="60"/>
       <c r="C53" s="60"/>
@@ -2250,9 +2611,41 @@
       <c r="K53" s="60"/>
       <c r="L53" s="60"/>
       <c r="M53" s="60"/>
+      <c r="N53" s="60"/>
+      <c r="O53" s="60"/>
+      <c r="P53" s="60"/>
+      <c r="Q53" s="60"/>
+      <c r="R53" s="60"/>
+      <c r="S53" s="60"/>
+      <c r="T53" s="60"/>
+      <c r="U53" s="60"/>
+      <c r="V53" s="60"/>
+      <c r="W53" s="60"/>
+      <c r="X53" s="60"/>
+      <c r="Y53" s="60"/>
+      <c r="Z53" s="60"/>
+      <c r="AA53" s="60"/>
+      <c r="AB53" s="60"/>
+      <c r="AC53" s="60"/>
+      <c r="AD53" s="60"/>
+      <c r="AE53" s="60"/>
+      <c r="AF53" s="60"/>
+      <c r="AG53" s="60"/>
+      <c r="AH53" s="60"/>
+      <c r="AI53" s="60"/>
+      <c r="AJ53" s="60"/>
+      <c r="AK53" s="60"/>
+      <c r="AL53" s="60"/>
+      <c r="AM53" s="60"/>
+      <c r="AN53" s="60"/>
+      <c r="AO53" s="60"/>
+      <c r="AP53" s="60"/>
+      <c r="AQ53" s="60"/>
+      <c r="AR53" s="60"/>
+      <c r="AS53" s="60"/>
       <c r="XFD53" s="60"/>
     </row>
-    <row r="54" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="54" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A54" s="60"/>
       <c r="B54" s="60"/>
       <c r="C54" s="60"/>
@@ -2266,9 +2659,41 @@
       <c r="K54" s="60"/>
       <c r="L54" s="60"/>
       <c r="M54" s="60"/>
+      <c r="N54" s="60"/>
+      <c r="O54" s="60"/>
+      <c r="P54" s="60"/>
+      <c r="Q54" s="60"/>
+      <c r="R54" s="60"/>
+      <c r="S54" s="60"/>
+      <c r="T54" s="60"/>
+      <c r="U54" s="60"/>
+      <c r="V54" s="60"/>
+      <c r="W54" s="60"/>
+      <c r="X54" s="60"/>
+      <c r="Y54" s="60"/>
+      <c r="Z54" s="60"/>
+      <c r="AA54" s="60"/>
+      <c r="AB54" s="60"/>
+      <c r="AC54" s="60"/>
+      <c r="AD54" s="60"/>
+      <c r="AE54" s="60"/>
+      <c r="AF54" s="60"/>
+      <c r="AG54" s="60"/>
+      <c r="AH54" s="60"/>
+      <c r="AI54" s="60"/>
+      <c r="AJ54" s="60"/>
+      <c r="AK54" s="60"/>
+      <c r="AL54" s="60"/>
+      <c r="AM54" s="60"/>
+      <c r="AN54" s="60"/>
+      <c r="AO54" s="60"/>
+      <c r="AP54" s="60"/>
+      <c r="AQ54" s="60"/>
+      <c r="AR54" s="60"/>
+      <c r="AS54" s="60"/>
       <c r="XFD54" s="60"/>
     </row>
-    <row r="55" spans="1:13 16384:16384" s="57" customFormat="1" ht="39">
+    <row r="55" spans="1:45 16384:16384" s="57" customFormat="1" ht="39">
       <c r="A55" s="60"/>
       <c r="B55" s="60"/>
       <c r="C55" s="60"/>
@@ -2280,9 +2705,43 @@
       <c r="I55" s="60"/>
       <c r="J55" s="60"/>
       <c r="K55" s="60"/>
+      <c r="L55" s="60"/>
+      <c r="M55" s="60"/>
+      <c r="N55" s="60"/>
+      <c r="O55" s="60"/>
+      <c r="P55" s="60"/>
+      <c r="Q55" s="60"/>
+      <c r="R55" s="60"/>
+      <c r="S55" s="60"/>
+      <c r="T55" s="60"/>
+      <c r="U55" s="60"/>
+      <c r="V55" s="60"/>
+      <c r="W55" s="60"/>
+      <c r="X55" s="60"/>
+      <c r="Y55" s="60"/>
+      <c r="Z55" s="60"/>
+      <c r="AA55" s="60"/>
+      <c r="AB55" s="60"/>
+      <c r="AC55" s="60"/>
+      <c r="AD55" s="60"/>
+      <c r="AE55" s="60"/>
+      <c r="AF55" s="60"/>
+      <c r="AG55" s="60"/>
+      <c r="AH55" s="60"/>
+      <c r="AI55" s="60"/>
+      <c r="AJ55" s="60"/>
+      <c r="AK55" s="60"/>
+      <c r="AL55" s="60"/>
+      <c r="AM55" s="60"/>
+      <c r="AN55" s="60"/>
+      <c r="AO55" s="60"/>
+      <c r="AP55" s="60"/>
+      <c r="AQ55" s="60"/>
+      <c r="AR55" s="60"/>
+      <c r="AS55" s="60"/>
       <c r="XFD55" s="60"/>
     </row>
-    <row r="56" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="56" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A56" s="60"/>
       <c r="B56" s="60"/>
       <c r="C56" s="60"/>
@@ -2296,9 +2755,41 @@
       <c r="K56" s="60"/>
       <c r="L56" s="60"/>
       <c r="M56" s="60"/>
+      <c r="N56" s="60"/>
+      <c r="O56" s="60"/>
+      <c r="P56" s="60"/>
+      <c r="Q56" s="60"/>
+      <c r="R56" s="60"/>
+      <c r="S56" s="60"/>
+      <c r="T56" s="60"/>
+      <c r="U56" s="60"/>
+      <c r="V56" s="60"/>
+      <c r="W56" s="60"/>
+      <c r="X56" s="60"/>
+      <c r="Y56" s="60"/>
+      <c r="Z56" s="60"/>
+      <c r="AA56" s="60"/>
+      <c r="AB56" s="60"/>
+      <c r="AC56" s="60"/>
+      <c r="AD56" s="60"/>
+      <c r="AE56" s="60"/>
+      <c r="AF56" s="60"/>
+      <c r="AG56" s="60"/>
+      <c r="AH56" s="60"/>
+      <c r="AI56" s="60"/>
+      <c r="AJ56" s="60"/>
+      <c r="AK56" s="60"/>
+      <c r="AL56" s="60"/>
+      <c r="AM56" s="60"/>
+      <c r="AN56" s="60"/>
+      <c r="AO56" s="60"/>
+      <c r="AP56" s="60"/>
+      <c r="AQ56" s="60"/>
+      <c r="AR56" s="60"/>
+      <c r="AS56" s="60"/>
       <c r="XFD56" s="60"/>
     </row>
-    <row r="57" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="57" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A57" s="60"/>
       <c r="B57" s="60"/>
       <c r="C57" s="60"/>
@@ -2312,9 +2803,41 @@
       <c r="K57" s="60"/>
       <c r="L57" s="60"/>
       <c r="M57" s="60"/>
+      <c r="N57" s="60"/>
+      <c r="O57" s="60"/>
+      <c r="P57" s="60"/>
+      <c r="Q57" s="60"/>
+      <c r="R57" s="60"/>
+      <c r="S57" s="60"/>
+      <c r="T57" s="60"/>
+      <c r="U57" s="60"/>
+      <c r="V57" s="60"/>
+      <c r="W57" s="60"/>
+      <c r="X57" s="60"/>
+      <c r="Y57" s="60"/>
+      <c r="Z57" s="60"/>
+      <c r="AA57" s="60"/>
+      <c r="AB57" s="60"/>
+      <c r="AC57" s="60"/>
+      <c r="AD57" s="60"/>
+      <c r="AE57" s="60"/>
+      <c r="AF57" s="60"/>
+      <c r="AG57" s="60"/>
+      <c r="AH57" s="60"/>
+      <c r="AI57" s="60"/>
+      <c r="AJ57" s="60"/>
+      <c r="AK57" s="60"/>
+      <c r="AL57" s="60"/>
+      <c r="AM57" s="60"/>
+      <c r="AN57" s="60"/>
+      <c r="AO57" s="60"/>
+      <c r="AP57" s="60"/>
+      <c r="AQ57" s="60"/>
+      <c r="AR57" s="60"/>
+      <c r="AS57" s="60"/>
       <c r="XFD57" s="60"/>
     </row>
-    <row r="58" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="58" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A58" s="60"/>
       <c r="B58" s="60"/>
       <c r="C58" s="60"/>
@@ -2328,9 +2851,41 @@
       <c r="K58" s="60"/>
       <c r="L58" s="60"/>
       <c r="M58" s="60"/>
+      <c r="N58" s="60"/>
+      <c r="O58" s="60"/>
+      <c r="P58" s="60"/>
+      <c r="Q58" s="60"/>
+      <c r="R58" s="60"/>
+      <c r="S58" s="60"/>
+      <c r="T58" s="60"/>
+      <c r="U58" s="60"/>
+      <c r="V58" s="60"/>
+      <c r="W58" s="60"/>
+      <c r="X58" s="60"/>
+      <c r="Y58" s="60"/>
+      <c r="Z58" s="60"/>
+      <c r="AA58" s="60"/>
+      <c r="AB58" s="60"/>
+      <c r="AC58" s="60"/>
+      <c r="AD58" s="60"/>
+      <c r="AE58" s="60"/>
+      <c r="AF58" s="60"/>
+      <c r="AG58" s="60"/>
+      <c r="AH58" s="60"/>
+      <c r="AI58" s="60"/>
+      <c r="AJ58" s="60"/>
+      <c r="AK58" s="60"/>
+      <c r="AL58" s="60"/>
+      <c r="AM58" s="60"/>
+      <c r="AN58" s="60"/>
+      <c r="AO58" s="60"/>
+      <c r="AP58" s="60"/>
+      <c r="AQ58" s="60"/>
+      <c r="AR58" s="60"/>
+      <c r="AS58" s="60"/>
       <c r="XFD58" s="60"/>
     </row>
-    <row r="59" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="59" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A59" s="60"/>
       <c r="B59" s="60"/>
       <c r="C59" s="60"/>
@@ -2344,9 +2899,41 @@
       <c r="K59" s="60"/>
       <c r="L59" s="60"/>
       <c r="M59" s="60"/>
+      <c r="N59" s="60"/>
+      <c r="O59" s="60"/>
+      <c r="P59" s="60"/>
+      <c r="Q59" s="60"/>
+      <c r="R59" s="60"/>
+      <c r="S59" s="60"/>
+      <c r="T59" s="60"/>
+      <c r="U59" s="60"/>
+      <c r="V59" s="60"/>
+      <c r="W59" s="60"/>
+      <c r="X59" s="60"/>
+      <c r="Y59" s="60"/>
+      <c r="Z59" s="60"/>
+      <c r="AA59" s="60"/>
+      <c r="AB59" s="60"/>
+      <c r="AC59" s="60"/>
+      <c r="AD59" s="60"/>
+      <c r="AE59" s="60"/>
+      <c r="AF59" s="60"/>
+      <c r="AG59" s="60"/>
+      <c r="AH59" s="60"/>
+      <c r="AI59" s="60"/>
+      <c r="AJ59" s="60"/>
+      <c r="AK59" s="60"/>
+      <c r="AL59" s="60"/>
+      <c r="AM59" s="60"/>
+      <c r="AN59" s="60"/>
+      <c r="AO59" s="60"/>
+      <c r="AP59" s="60"/>
+      <c r="AQ59" s="60"/>
+      <c r="AR59" s="60"/>
+      <c r="AS59" s="60"/>
       <c r="XFD59" s="60"/>
     </row>
-    <row r="60" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="60" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A60" s="60"/>
       <c r="B60" s="60"/>
       <c r="C60" s="60"/>
@@ -2360,9 +2947,41 @@
       <c r="K60" s="60"/>
       <c r="L60" s="60"/>
       <c r="M60" s="60"/>
+      <c r="N60" s="60"/>
+      <c r="O60" s="60"/>
+      <c r="P60" s="60"/>
+      <c r="Q60" s="60"/>
+      <c r="R60" s="60"/>
+      <c r="S60" s="60"/>
+      <c r="T60" s="60"/>
+      <c r="U60" s="60"/>
+      <c r="V60" s="60"/>
+      <c r="W60" s="60"/>
+      <c r="X60" s="60"/>
+      <c r="Y60" s="60"/>
+      <c r="Z60" s="60"/>
+      <c r="AA60" s="60"/>
+      <c r="AB60" s="60"/>
+      <c r="AC60" s="60"/>
+      <c r="AD60" s="60"/>
+      <c r="AE60" s="60"/>
+      <c r="AF60" s="60"/>
+      <c r="AG60" s="60"/>
+      <c r="AH60" s="60"/>
+      <c r="AI60" s="60"/>
+      <c r="AJ60" s="60"/>
+      <c r="AK60" s="60"/>
+      <c r="AL60" s="60"/>
+      <c r="AM60" s="60"/>
+      <c r="AN60" s="60"/>
+      <c r="AO60" s="60"/>
+      <c r="AP60" s="60"/>
+      <c r="AQ60" s="60"/>
+      <c r="AR60" s="60"/>
+      <c r="AS60" s="60"/>
       <c r="XFD60" s="60"/>
     </row>
-    <row r="61" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="61" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A61" s="60"/>
       <c r="B61" s="60"/>
       <c r="C61" s="60"/>
@@ -2376,9 +2995,41 @@
       <c r="K61" s="60"/>
       <c r="L61" s="60"/>
       <c r="M61" s="60"/>
+      <c r="N61" s="60"/>
+      <c r="O61" s="60"/>
+      <c r="P61" s="60"/>
+      <c r="Q61" s="60"/>
+      <c r="R61" s="60"/>
+      <c r="S61" s="60"/>
+      <c r="T61" s="60"/>
+      <c r="U61" s="60"/>
+      <c r="V61" s="60"/>
+      <c r="W61" s="60"/>
+      <c r="X61" s="60"/>
+      <c r="Y61" s="60"/>
+      <c r="Z61" s="60"/>
+      <c r="AA61" s="60"/>
+      <c r="AB61" s="60"/>
+      <c r="AC61" s="60"/>
+      <c r="AD61" s="60"/>
+      <c r="AE61" s="60"/>
+      <c r="AF61" s="60"/>
+      <c r="AG61" s="60"/>
+      <c r="AH61" s="60"/>
+      <c r="AI61" s="60"/>
+      <c r="AJ61" s="60"/>
+      <c r="AK61" s="60"/>
+      <c r="AL61" s="60"/>
+      <c r="AM61" s="60"/>
+      <c r="AN61" s="60"/>
+      <c r="AO61" s="60"/>
+      <c r="AP61" s="60"/>
+      <c r="AQ61" s="60"/>
+      <c r="AR61" s="60"/>
+      <c r="AS61" s="60"/>
       <c r="XFD61" s="60"/>
     </row>
-    <row r="62" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="62" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A62" s="60"/>
       <c r="B62" s="60"/>
       <c r="C62" s="60"/>
@@ -2392,9 +3043,41 @@
       <c r="K62" s="60"/>
       <c r="L62" s="60"/>
       <c r="M62" s="60"/>
+      <c r="N62" s="60"/>
+      <c r="O62" s="60"/>
+      <c r="P62" s="60"/>
+      <c r="Q62" s="60"/>
+      <c r="R62" s="60"/>
+      <c r="S62" s="60"/>
+      <c r="T62" s="60"/>
+      <c r="U62" s="60"/>
+      <c r="V62" s="60"/>
+      <c r="W62" s="60"/>
+      <c r="X62" s="60"/>
+      <c r="Y62" s="60"/>
+      <c r="Z62" s="60"/>
+      <c r="AA62" s="60"/>
+      <c r="AB62" s="60"/>
+      <c r="AC62" s="60"/>
+      <c r="AD62" s="60"/>
+      <c r="AE62" s="60"/>
+      <c r="AF62" s="60"/>
+      <c r="AG62" s="60"/>
+      <c r="AH62" s="60"/>
+      <c r="AI62" s="60"/>
+      <c r="AJ62" s="60"/>
+      <c r="AK62" s="60"/>
+      <c r="AL62" s="60"/>
+      <c r="AM62" s="60"/>
+      <c r="AN62" s="60"/>
+      <c r="AO62" s="60"/>
+      <c r="AP62" s="60"/>
+      <c r="AQ62" s="60"/>
+      <c r="AR62" s="60"/>
+      <c r="AS62" s="60"/>
       <c r="XFD62" s="60"/>
     </row>
-    <row r="63" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="63" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A63" s="60"/>
       <c r="B63" s="60"/>
       <c r="C63" s="60"/>
@@ -2402,12 +3085,47 @@
       <c r="E63" s="60"/>
       <c r="F63" s="60"/>
       <c r="G63" s="60"/>
+      <c r="H63" s="60"/>
+      <c r="I63" s="60"/>
       <c r="J63" s="60"/>
       <c r="K63" s="60"/>
       <c r="L63" s="60"/>
+      <c r="M63" s="60"/>
+      <c r="N63" s="60"/>
+      <c r="O63" s="60"/>
+      <c r="P63" s="60"/>
+      <c r="Q63" s="60"/>
+      <c r="R63" s="60"/>
+      <c r="S63" s="60"/>
+      <c r="T63" s="60"/>
+      <c r="U63" s="60"/>
+      <c r="V63" s="60"/>
+      <c r="W63" s="60"/>
+      <c r="X63" s="60"/>
+      <c r="Y63" s="60"/>
+      <c r="Z63" s="60"/>
+      <c r="AA63" s="60"/>
+      <c r="AB63" s="60"/>
+      <c r="AC63" s="60"/>
+      <c r="AD63" s="60"/>
+      <c r="AE63" s="60"/>
+      <c r="AF63" s="60"/>
+      <c r="AG63" s="60"/>
+      <c r="AH63" s="60"/>
+      <c r="AI63" s="60"/>
+      <c r="AJ63" s="60"/>
+      <c r="AK63" s="60"/>
+      <c r="AL63" s="60"/>
+      <c r="AM63" s="60"/>
+      <c r="AN63" s="60"/>
+      <c r="AO63" s="60"/>
+      <c r="AP63" s="60"/>
+      <c r="AQ63" s="60"/>
+      <c r="AR63" s="60"/>
+      <c r="AS63" s="60"/>
       <c r="XFD63" s="60"/>
     </row>
-    <row r="64" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="64" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A64" s="60"/>
       <c r="B64" s="60"/>
       <c r="C64" s="60"/>
@@ -2415,12 +3133,47 @@
       <c r="E64" s="60"/>
       <c r="F64" s="60"/>
       <c r="G64" s="60"/>
+      <c r="H64" s="60"/>
+      <c r="I64" s="60"/>
       <c r="J64" s="60"/>
       <c r="K64" s="60"/>
       <c r="L64" s="60"/>
+      <c r="M64" s="60"/>
+      <c r="N64" s="60"/>
+      <c r="O64" s="60"/>
+      <c r="P64" s="60"/>
+      <c r="Q64" s="60"/>
+      <c r="R64" s="60"/>
+      <c r="S64" s="60"/>
+      <c r="T64" s="60"/>
+      <c r="U64" s="60"/>
+      <c r="V64" s="60"/>
+      <c r="W64" s="60"/>
+      <c r="X64" s="60"/>
+      <c r="Y64" s="60"/>
+      <c r="Z64" s="60"/>
+      <c r="AA64" s="60"/>
+      <c r="AB64" s="60"/>
+      <c r="AC64" s="60"/>
+      <c r="AD64" s="60"/>
+      <c r="AE64" s="60"/>
+      <c r="AF64" s="60"/>
+      <c r="AG64" s="60"/>
+      <c r="AH64" s="60"/>
+      <c r="AI64" s="60"/>
+      <c r="AJ64" s="60"/>
+      <c r="AK64" s="60"/>
+      <c r="AL64" s="60"/>
+      <c r="AM64" s="60"/>
+      <c r="AN64" s="60"/>
+      <c r="AO64" s="60"/>
+      <c r="AP64" s="60"/>
+      <c r="AQ64" s="60"/>
+      <c r="AR64" s="60"/>
+      <c r="AS64" s="60"/>
       <c r="XFD64" s="60"/>
     </row>
-    <row r="65" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="65" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A65" s="60"/>
       <c r="B65" s="60"/>
       <c r="C65" s="60"/>
@@ -2428,12 +3181,47 @@
       <c r="E65" s="60"/>
       <c r="F65" s="60"/>
       <c r="G65" s="60"/>
+      <c r="H65" s="60"/>
+      <c r="I65" s="60"/>
       <c r="J65" s="60"/>
       <c r="K65" s="60"/>
       <c r="L65" s="60"/>
+      <c r="M65" s="60"/>
+      <c r="N65" s="60"/>
+      <c r="O65" s="60"/>
+      <c r="P65" s="60"/>
+      <c r="Q65" s="60"/>
+      <c r="R65" s="60"/>
+      <c r="S65" s="60"/>
+      <c r="T65" s="60"/>
+      <c r="U65" s="60"/>
+      <c r="V65" s="60"/>
+      <c r="W65" s="60"/>
+      <c r="X65" s="60"/>
+      <c r="Y65" s="60"/>
+      <c r="Z65" s="60"/>
+      <c r="AA65" s="60"/>
+      <c r="AB65" s="60"/>
+      <c r="AC65" s="60"/>
+      <c r="AD65" s="60"/>
+      <c r="AE65" s="60"/>
+      <c r="AF65" s="60"/>
+      <c r="AG65" s="60"/>
+      <c r="AH65" s="60"/>
+      <c r="AI65" s="60"/>
+      <c r="AJ65" s="60"/>
+      <c r="AK65" s="60"/>
+      <c r="AL65" s="60"/>
+      <c r="AM65" s="60"/>
+      <c r="AN65" s="60"/>
+      <c r="AO65" s="60"/>
+      <c r="AP65" s="60"/>
+      <c r="AQ65" s="60"/>
+      <c r="AR65" s="60"/>
+      <c r="AS65" s="60"/>
       <c r="XFD65" s="60"/>
     </row>
-    <row r="66" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="66" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A66" s="60"/>
       <c r="B66" s="60"/>
       <c r="C66" s="60"/>
@@ -2447,9 +3235,41 @@
       <c r="K66" s="60"/>
       <c r="L66" s="60"/>
       <c r="M66" s="60"/>
+      <c r="N66" s="60"/>
+      <c r="O66" s="60"/>
+      <c r="P66" s="60"/>
+      <c r="Q66" s="60"/>
+      <c r="R66" s="60"/>
+      <c r="S66" s="60"/>
+      <c r="T66" s="60"/>
+      <c r="U66" s="60"/>
+      <c r="V66" s="60"/>
+      <c r="W66" s="60"/>
+      <c r="X66" s="60"/>
+      <c r="Y66" s="60"/>
+      <c r="Z66" s="60"/>
+      <c r="AA66" s="60"/>
+      <c r="AB66" s="60"/>
+      <c r="AC66" s="60"/>
+      <c r="AD66" s="60"/>
+      <c r="AE66" s="60"/>
+      <c r="AF66" s="60"/>
+      <c r="AG66" s="60"/>
+      <c r="AH66" s="60"/>
+      <c r="AI66" s="60"/>
+      <c r="AJ66" s="60"/>
+      <c r="AK66" s="60"/>
+      <c r="AL66" s="60"/>
+      <c r="AM66" s="60"/>
+      <c r="AN66" s="60"/>
+      <c r="AO66" s="60"/>
+      <c r="AP66" s="60"/>
+      <c r="AQ66" s="60"/>
+      <c r="AR66" s="60"/>
+      <c r="AS66" s="60"/>
       <c r="XFD66" s="60"/>
     </row>
-    <row r="67" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="67" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A67" s="60"/>
       <c r="B67" s="60"/>
       <c r="C67" s="60"/>
@@ -2463,9 +3283,41 @@
       <c r="K67" s="60"/>
       <c r="L67" s="60"/>
       <c r="M67" s="60"/>
+      <c r="N67" s="60"/>
+      <c r="O67" s="60"/>
+      <c r="P67" s="60"/>
+      <c r="Q67" s="60"/>
+      <c r="R67" s="60"/>
+      <c r="S67" s="60"/>
+      <c r="T67" s="60"/>
+      <c r="U67" s="60"/>
+      <c r="V67" s="60"/>
+      <c r="W67" s="60"/>
+      <c r="X67" s="60"/>
+      <c r="Y67" s="60"/>
+      <c r="Z67" s="60"/>
+      <c r="AA67" s="60"/>
+      <c r="AB67" s="60"/>
+      <c r="AC67" s="60"/>
+      <c r="AD67" s="60"/>
+      <c r="AE67" s="60"/>
+      <c r="AF67" s="60"/>
+      <c r="AG67" s="60"/>
+      <c r="AH67" s="60"/>
+      <c r="AI67" s="60"/>
+      <c r="AJ67" s="60"/>
+      <c r="AK67" s="60"/>
+      <c r="AL67" s="60"/>
+      <c r="AM67" s="60"/>
+      <c r="AN67" s="60"/>
+      <c r="AO67" s="60"/>
+      <c r="AP67" s="60"/>
+      <c r="AQ67" s="60"/>
+      <c r="AR67" s="60"/>
+      <c r="AS67" s="60"/>
       <c r="XFD67" s="60"/>
     </row>
-    <row r="68" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="68" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A68" s="60"/>
       <c r="B68" s="60"/>
       <c r="C68" s="60"/>
@@ -2479,9 +3331,41 @@
       <c r="K68" s="60"/>
       <c r="L68" s="60"/>
       <c r="M68" s="60"/>
+      <c r="N68" s="60"/>
+      <c r="O68" s="60"/>
+      <c r="P68" s="60"/>
+      <c r="Q68" s="60"/>
+      <c r="R68" s="60"/>
+      <c r="S68" s="60"/>
+      <c r="T68" s="60"/>
+      <c r="U68" s="60"/>
+      <c r="V68" s="60"/>
+      <c r="W68" s="60"/>
+      <c r="X68" s="60"/>
+      <c r="Y68" s="60"/>
+      <c r="Z68" s="60"/>
+      <c r="AA68" s="60"/>
+      <c r="AB68" s="60"/>
+      <c r="AC68" s="60"/>
+      <c r="AD68" s="60"/>
+      <c r="AE68" s="60"/>
+      <c r="AF68" s="60"/>
+      <c r="AG68" s="60"/>
+      <c r="AH68" s="60"/>
+      <c r="AI68" s="60"/>
+      <c r="AJ68" s="60"/>
+      <c r="AK68" s="60"/>
+      <c r="AL68" s="60"/>
+      <c r="AM68" s="60"/>
+      <c r="AN68" s="60"/>
+      <c r="AO68" s="60"/>
+      <c r="AP68" s="60"/>
+      <c r="AQ68" s="60"/>
+      <c r="AR68" s="60"/>
+      <c r="AS68" s="60"/>
       <c r="XFD68" s="60"/>
     </row>
-    <row r="69" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="69" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A69" s="60"/>
       <c r="B69" s="60"/>
       <c r="C69" s="60"/>
@@ -2495,9 +3379,41 @@
       <c r="K69" s="60"/>
       <c r="L69" s="60"/>
       <c r="M69" s="60"/>
+      <c r="N69" s="60"/>
+      <c r="O69" s="60"/>
+      <c r="P69" s="60"/>
+      <c r="Q69" s="60"/>
+      <c r="R69" s="60"/>
+      <c r="S69" s="60"/>
+      <c r="T69" s="60"/>
+      <c r="U69" s="60"/>
+      <c r="V69" s="60"/>
+      <c r="W69" s="60"/>
+      <c r="X69" s="60"/>
+      <c r="Y69" s="60"/>
+      <c r="Z69" s="60"/>
+      <c r="AA69" s="60"/>
+      <c r="AB69" s="60"/>
+      <c r="AC69" s="60"/>
+      <c r="AD69" s="60"/>
+      <c r="AE69" s="60"/>
+      <c r="AF69" s="60"/>
+      <c r="AG69" s="60"/>
+      <c r="AH69" s="60"/>
+      <c r="AI69" s="60"/>
+      <c r="AJ69" s="60"/>
+      <c r="AK69" s="60"/>
+      <c r="AL69" s="60"/>
+      <c r="AM69" s="60"/>
+      <c r="AN69" s="60"/>
+      <c r="AO69" s="60"/>
+      <c r="AP69" s="60"/>
+      <c r="AQ69" s="60"/>
+      <c r="AR69" s="60"/>
+      <c r="AS69" s="60"/>
       <c r="XFD69" s="60"/>
     </row>
-    <row r="70" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="70" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A70" s="60"/>
       <c r="B70" s="60"/>
       <c r="C70" s="60"/>
@@ -2505,12 +3421,47 @@
       <c r="E70" s="60"/>
       <c r="F70" s="60"/>
       <c r="G70" s="60"/>
+      <c r="H70" s="60"/>
+      <c r="I70" s="60"/>
       <c r="J70" s="60"/>
       <c r="K70" s="60"/>
       <c r="L70" s="60"/>
+      <c r="M70" s="60"/>
+      <c r="N70" s="60"/>
+      <c r="O70" s="60"/>
+      <c r="P70" s="60"/>
+      <c r="Q70" s="60"/>
+      <c r="R70" s="60"/>
+      <c r="S70" s="60"/>
+      <c r="T70" s="60"/>
+      <c r="U70" s="60"/>
+      <c r="V70" s="60"/>
+      <c r="W70" s="60"/>
+      <c r="X70" s="60"/>
+      <c r="Y70" s="60"/>
+      <c r="Z70" s="60"/>
+      <c r="AA70" s="60"/>
+      <c r="AB70" s="60"/>
+      <c r="AC70" s="60"/>
+      <c r="AD70" s="60"/>
+      <c r="AE70" s="60"/>
+      <c r="AF70" s="60"/>
+      <c r="AG70" s="60"/>
+      <c r="AH70" s="60"/>
+      <c r="AI70" s="60"/>
+      <c r="AJ70" s="60"/>
+      <c r="AK70" s="60"/>
+      <c r="AL70" s="60"/>
+      <c r="AM70" s="60"/>
+      <c r="AN70" s="60"/>
+      <c r="AO70" s="60"/>
+      <c r="AP70" s="60"/>
+      <c r="AQ70" s="60"/>
+      <c r="AR70" s="60"/>
+      <c r="AS70" s="60"/>
       <c r="XFD70" s="60"/>
     </row>
-    <row r="71" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="71" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A71" s="60"/>
       <c r="B71" s="60"/>
       <c r="C71" s="60"/>
@@ -2518,12 +3469,47 @@
       <c r="E71" s="60"/>
       <c r="F71" s="60"/>
       <c r="G71" s="60"/>
+      <c r="H71" s="60"/>
+      <c r="I71" s="60"/>
       <c r="J71" s="60"/>
       <c r="K71" s="60"/>
       <c r="L71" s="60"/>
+      <c r="M71" s="60"/>
+      <c r="N71" s="60"/>
+      <c r="O71" s="60"/>
+      <c r="P71" s="60"/>
+      <c r="Q71" s="60"/>
+      <c r="R71" s="60"/>
+      <c r="S71" s="60"/>
+      <c r="T71" s="60"/>
+      <c r="U71" s="60"/>
+      <c r="V71" s="60"/>
+      <c r="W71" s="60"/>
+      <c r="X71" s="60"/>
+      <c r="Y71" s="60"/>
+      <c r="Z71" s="60"/>
+      <c r="AA71" s="60"/>
+      <c r="AB71" s="60"/>
+      <c r="AC71" s="60"/>
+      <c r="AD71" s="60"/>
+      <c r="AE71" s="60"/>
+      <c r="AF71" s="60"/>
+      <c r="AG71" s="60"/>
+      <c r="AH71" s="60"/>
+      <c r="AI71" s="60"/>
+      <c r="AJ71" s="60"/>
+      <c r="AK71" s="60"/>
+      <c r="AL71" s="60"/>
+      <c r="AM71" s="60"/>
+      <c r="AN71" s="60"/>
+      <c r="AO71" s="60"/>
+      <c r="AP71" s="60"/>
+      <c r="AQ71" s="60"/>
+      <c r="AR71" s="60"/>
+      <c r="AS71" s="60"/>
       <c r="XFD71" s="60"/>
     </row>
-    <row r="72" spans="1:13 16384:16384" s="56" customFormat="1" ht="39">
+    <row r="72" spans="1:45 16384:16384" s="56" customFormat="1" ht="39">
       <c r="A72" s="60"/>
       <c r="B72" s="60"/>
       <c r="C72" s="60"/>
@@ -2531,12 +3517,47 @@
       <c r="E72" s="60"/>
       <c r="F72" s="60"/>
       <c r="G72" s="60"/>
+      <c r="H72" s="60"/>
+      <c r="I72" s="60"/>
       <c r="J72" s="60"/>
       <c r="K72" s="60"/>
       <c r="L72" s="60"/>
+      <c r="M72" s="60"/>
+      <c r="N72" s="60"/>
+      <c r="O72" s="60"/>
+      <c r="P72" s="60"/>
+      <c r="Q72" s="60"/>
+      <c r="R72" s="60"/>
+      <c r="S72" s="60"/>
+      <c r="T72" s="60"/>
+      <c r="U72" s="60"/>
+      <c r="V72" s="60"/>
+      <c r="W72" s="60"/>
+      <c r="X72" s="60"/>
+      <c r="Y72" s="60"/>
+      <c r="Z72" s="60"/>
+      <c r="AA72" s="60"/>
+      <c r="AB72" s="60"/>
+      <c r="AC72" s="60"/>
+      <c r="AD72" s="60"/>
+      <c r="AE72" s="60"/>
+      <c r="AF72" s="60"/>
+      <c r="AG72" s="60"/>
+      <c r="AH72" s="60"/>
+      <c r="AI72" s="60"/>
+      <c r="AJ72" s="60"/>
+      <c r="AK72" s="60"/>
+      <c r="AL72" s="60"/>
+      <c r="AM72" s="60"/>
+      <c r="AN72" s="60"/>
+      <c r="AO72" s="60"/>
+      <c r="AP72" s="60"/>
+      <c r="AQ72" s="60"/>
+      <c r="AR72" s="60"/>
+      <c r="AS72" s="60"/>
       <c r="XFD72" s="60"/>
     </row>
-    <row r="73" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="73" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A73" s="60"/>
       <c r="B73" s="60"/>
       <c r="C73" s="60"/>
@@ -2550,9 +3571,41 @@
       <c r="K73" s="60"/>
       <c r="L73" s="60"/>
       <c r="M73" s="60"/>
+      <c r="N73" s="60"/>
+      <c r="O73" s="60"/>
+      <c r="P73" s="60"/>
+      <c r="Q73" s="60"/>
+      <c r="R73" s="60"/>
+      <c r="S73" s="60"/>
+      <c r="T73" s="60"/>
+      <c r="U73" s="60"/>
+      <c r="V73" s="60"/>
+      <c r="W73" s="60"/>
+      <c r="X73" s="60"/>
+      <c r="Y73" s="60"/>
+      <c r="Z73" s="60"/>
+      <c r="AA73" s="60"/>
+      <c r="AB73" s="60"/>
+      <c r="AC73" s="60"/>
+      <c r="AD73" s="60"/>
+      <c r="AE73" s="60"/>
+      <c r="AF73" s="60"/>
+      <c r="AG73" s="60"/>
+      <c r="AH73" s="60"/>
+      <c r="AI73" s="60"/>
+      <c r="AJ73" s="60"/>
+      <c r="AK73" s="60"/>
+      <c r="AL73" s="60"/>
+      <c r="AM73" s="60"/>
+      <c r="AN73" s="60"/>
+      <c r="AO73" s="60"/>
+      <c r="AP73" s="60"/>
+      <c r="AQ73" s="60"/>
+      <c r="AR73" s="60"/>
+      <c r="AS73" s="60"/>
       <c r="XFD73" s="60"/>
     </row>
-    <row r="74" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="74" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A74" s="60"/>
       <c r="B74" s="60"/>
       <c r="C74" s="60"/>
@@ -2566,9 +3619,41 @@
       <c r="K74" s="60"/>
       <c r="L74" s="60"/>
       <c r="M74" s="60"/>
+      <c r="N74" s="60"/>
+      <c r="O74" s="60"/>
+      <c r="P74" s="60"/>
+      <c r="Q74" s="60"/>
+      <c r="R74" s="60"/>
+      <c r="S74" s="60"/>
+      <c r="T74" s="60"/>
+      <c r="U74" s="60"/>
+      <c r="V74" s="60"/>
+      <c r="W74" s="60"/>
+      <c r="X74" s="60"/>
+      <c r="Y74" s="60"/>
+      <c r="Z74" s="60"/>
+      <c r="AA74" s="60"/>
+      <c r="AB74" s="60"/>
+      <c r="AC74" s="60"/>
+      <c r="AD74" s="60"/>
+      <c r="AE74" s="60"/>
+      <c r="AF74" s="60"/>
+      <c r="AG74" s="60"/>
+      <c r="AH74" s="60"/>
+      <c r="AI74" s="60"/>
+      <c r="AJ74" s="60"/>
+      <c r="AK74" s="60"/>
+      <c r="AL74" s="60"/>
+      <c r="AM74" s="60"/>
+      <c r="AN74" s="60"/>
+      <c r="AO74" s="60"/>
+      <c r="AP74" s="60"/>
+      <c r="AQ74" s="60"/>
+      <c r="AR74" s="60"/>
+      <c r="AS74" s="60"/>
       <c r="XFD74" s="60"/>
     </row>
-    <row r="75" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="75" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A75" s="60"/>
       <c r="B75" s="60"/>
       <c r="C75" s="60"/>
@@ -2582,9 +3667,41 @@
       <c r="K75" s="60"/>
       <c r="L75" s="60"/>
       <c r="M75" s="60"/>
+      <c r="N75" s="60"/>
+      <c r="O75" s="60"/>
+      <c r="P75" s="60"/>
+      <c r="Q75" s="60"/>
+      <c r="R75" s="60"/>
+      <c r="S75" s="60"/>
+      <c r="T75" s="60"/>
+      <c r="U75" s="60"/>
+      <c r="V75" s="60"/>
+      <c r="W75" s="60"/>
+      <c r="X75" s="60"/>
+      <c r="Y75" s="60"/>
+      <c r="Z75" s="60"/>
+      <c r="AA75" s="60"/>
+      <c r="AB75" s="60"/>
+      <c r="AC75" s="60"/>
+      <c r="AD75" s="60"/>
+      <c r="AE75" s="60"/>
+      <c r="AF75" s="60"/>
+      <c r="AG75" s="60"/>
+      <c r="AH75" s="60"/>
+      <c r="AI75" s="60"/>
+      <c r="AJ75" s="60"/>
+      <c r="AK75" s="60"/>
+      <c r="AL75" s="60"/>
+      <c r="AM75" s="60"/>
+      <c r="AN75" s="60"/>
+      <c r="AO75" s="60"/>
+      <c r="AP75" s="60"/>
+      <c r="AQ75" s="60"/>
+      <c r="AR75" s="60"/>
+      <c r="AS75" s="60"/>
       <c r="XFD75" s="60"/>
     </row>
-    <row r="76" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="76" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A76" s="60"/>
       <c r="B76" s="60"/>
       <c r="C76" s="60"/>
@@ -2598,9 +3715,41 @@
       <c r="K76" s="60"/>
       <c r="L76" s="60"/>
       <c r="M76" s="60"/>
+      <c r="N76" s="60"/>
+      <c r="O76" s="60"/>
+      <c r="P76" s="60"/>
+      <c r="Q76" s="60"/>
+      <c r="R76" s="60"/>
+      <c r="S76" s="60"/>
+      <c r="T76" s="60"/>
+      <c r="U76" s="60"/>
+      <c r="V76" s="60"/>
+      <c r="W76" s="60"/>
+      <c r="X76" s="60"/>
+      <c r="Y76" s="60"/>
+      <c r="Z76" s="60"/>
+      <c r="AA76" s="60"/>
+      <c r="AB76" s="60"/>
+      <c r="AC76" s="60"/>
+      <c r="AD76" s="60"/>
+      <c r="AE76" s="60"/>
+      <c r="AF76" s="60"/>
+      <c r="AG76" s="60"/>
+      <c r="AH76" s="60"/>
+      <c r="AI76" s="60"/>
+      <c r="AJ76" s="60"/>
+      <c r="AK76" s="60"/>
+      <c r="AL76" s="60"/>
+      <c r="AM76" s="60"/>
+      <c r="AN76" s="60"/>
+      <c r="AO76" s="60"/>
+      <c r="AP76" s="60"/>
+      <c r="AQ76" s="60"/>
+      <c r="AR76" s="60"/>
+      <c r="AS76" s="60"/>
       <c r="XFD76" s="60"/>
     </row>
-    <row r="77" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="77" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A77" s="60"/>
       <c r="B77" s="60"/>
       <c r="C77" s="60"/>
@@ -2614,9 +3763,41 @@
       <c r="K77" s="60"/>
       <c r="L77" s="60"/>
       <c r="M77" s="60"/>
+      <c r="N77" s="60"/>
+      <c r="O77" s="60"/>
+      <c r="P77" s="60"/>
+      <c r="Q77" s="60"/>
+      <c r="R77" s="60"/>
+      <c r="S77" s="60"/>
+      <c r="T77" s="60"/>
+      <c r="U77" s="60"/>
+      <c r="V77" s="60"/>
+      <c r="W77" s="60"/>
+      <c r="X77" s="60"/>
+      <c r="Y77" s="60"/>
+      <c r="Z77" s="60"/>
+      <c r="AA77" s="60"/>
+      <c r="AB77" s="60"/>
+      <c r="AC77" s="60"/>
+      <c r="AD77" s="60"/>
+      <c r="AE77" s="60"/>
+      <c r="AF77" s="60"/>
+      <c r="AG77" s="60"/>
+      <c r="AH77" s="60"/>
+      <c r="AI77" s="60"/>
+      <c r="AJ77" s="60"/>
+      <c r="AK77" s="60"/>
+      <c r="AL77" s="60"/>
+      <c r="AM77" s="60"/>
+      <c r="AN77" s="60"/>
+      <c r="AO77" s="60"/>
+      <c r="AP77" s="60"/>
+      <c r="AQ77" s="60"/>
+      <c r="AR77" s="60"/>
+      <c r="AS77" s="60"/>
       <c r="XFD77" s="60"/>
     </row>
-    <row r="78" spans="1:13 16384:16384" s="59" customFormat="1" ht="31.5">
+    <row r="78" spans="1:45 16384:16384" s="59" customFormat="1" ht="31.5">
       <c r="A78" s="60"/>
       <c r="B78" s="60"/>
       <c r="C78" s="60"/>
@@ -2626,9 +3807,45 @@
       <c r="G78" s="60"/>
       <c r="H78" s="60"/>
       <c r="I78" s="60"/>
+      <c r="J78" s="60"/>
+      <c r="K78" s="60"/>
+      <c r="L78" s="60"/>
+      <c r="M78" s="60"/>
+      <c r="N78" s="60"/>
+      <c r="O78" s="60"/>
+      <c r="P78" s="60"/>
+      <c r="Q78" s="60"/>
+      <c r="R78" s="60"/>
+      <c r="S78" s="60"/>
+      <c r="T78" s="60"/>
+      <c r="U78" s="60"/>
+      <c r="V78" s="60"/>
+      <c r="W78" s="60"/>
+      <c r="X78" s="60"/>
+      <c r="Y78" s="60"/>
+      <c r="Z78" s="60"/>
+      <c r="AA78" s="60"/>
+      <c r="AB78" s="60"/>
+      <c r="AC78" s="60"/>
+      <c r="AD78" s="60"/>
+      <c r="AE78" s="60"/>
+      <c r="AF78" s="60"/>
+      <c r="AG78" s="60"/>
+      <c r="AH78" s="60"/>
+      <c r="AI78" s="60"/>
+      <c r="AJ78" s="60"/>
+      <c r="AK78" s="60"/>
+      <c r="AL78" s="60"/>
+      <c r="AM78" s="60"/>
+      <c r="AN78" s="60"/>
+      <c r="AO78" s="60"/>
+      <c r="AP78" s="60"/>
+      <c r="AQ78" s="60"/>
+      <c r="AR78" s="60"/>
+      <c r="AS78" s="60"/>
       <c r="XFD78" s="60"/>
     </row>
-    <row r="79" spans="1:13 16384:16384" s="58" customFormat="1">
+    <row r="79" spans="1:45 16384:16384" s="58" customFormat="1">
       <c r="A79" s="60"/>
       <c r="B79" s="60"/>
       <c r="C79" s="60"/>
@@ -2642,14 +3859,40 @@
       <c r="K79" s="60"/>
       <c r="L79" s="60"/>
       <c r="M79" s="60"/>
+      <c r="N79" s="60"/>
+      <c r="O79" s="60"/>
+      <c r="P79" s="60"/>
+      <c r="Q79" s="60"/>
+      <c r="R79" s="60"/>
+      <c r="S79" s="60"/>
+      <c r="T79" s="60"/>
+      <c r="U79" s="60"/>
+      <c r="V79" s="60"/>
+      <c r="W79" s="60"/>
+      <c r="X79" s="60"/>
+      <c r="Y79" s="60"/>
+      <c r="Z79" s="60"/>
+      <c r="AA79" s="60"/>
+      <c r="AB79" s="60"/>
+      <c r="AC79" s="60"/>
+      <c r="AD79" s="60"/>
+      <c r="AE79" s="60"/>
+      <c r="AF79" s="60"/>
+      <c r="AG79" s="60"/>
+      <c r="AH79" s="60"/>
+      <c r="AI79" s="60"/>
+      <c r="AJ79" s="60"/>
+      <c r="AK79" s="60"/>
+      <c r="AL79" s="60"/>
+      <c r="AM79" s="60"/>
+      <c r="AN79" s="60"/>
+      <c r="AO79" s="60"/>
+      <c r="AP79" s="60"/>
+      <c r="AQ79" s="60"/>
+      <c r="AR79" s="60"/>
+      <c r="AS79" s="60"/>
       <c r="XFD79" s="60"/>
     </row>
-    <row r="82" s="60" customFormat="1"/>
-    <row r="83" s="60" customFormat="1"/>
-    <row r="84" s="60" customFormat="1"/>
-    <row r="85" s="60" customFormat="1"/>
-    <row r="86" s="60" customFormat="1"/>
-    <row r="87" s="60" customFormat="1"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="E24:G24"/>
@@ -2663,7 +3906,6 @@
   </mergeCells>
   <pageMargins left="1.0625" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="42" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2671,8 +3913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -2691,70 +3933,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="93" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
+      <c r="B4" s="93"/>
+      <c r="C4" s="93"/>
+      <c r="D4" s="93"/>
+      <c r="E4" s="93"/>
+      <c r="F4" s="93"/>
+      <c r="G4" s="93"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
     </row>
     <row r="6" spans="1:7" ht="69" customHeight="1">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="96" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="6"/>
@@ -2857,12 +4099,12 @@
     </row>
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="35"/>
-      <c r="B15" s="93" t="s">
+      <c r="B15" s="97" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="93"/>
-      <c r="D15" s="93"/>
-      <c r="E15" s="93"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
       <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:7" ht="25.5" customHeight="1">
@@ -2930,11 +4172,11 @@
       <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:7" ht="42" customHeight="1">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="98"/>
       <c r="D23" s="24"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -2944,47 +4186,47 @@
       <c r="A24" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="95" t="s">
+      <c r="B24" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="95"/>
+      <c r="C24" s="99"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="6"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="44.1" customHeight="1">
-      <c r="A25" s="96" t="s">
+      <c r="A25" s="100" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="91" t="s">
+      <c r="A27" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
     </row>
     <row r="28" spans="1:7" ht="42" customHeight="1">
       <c r="E28" s="35"/>
@@ -3036,11 +4278,6 @@
     <row r="63" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A6:G6"/>
@@ -3048,6 +4285,11 @@
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -3056,7 +4298,6 @@
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3064,8 +4305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A4" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28:L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -3090,92 +4331,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A1" s="97" t="s">
+      <c r="A1" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="97"/>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="91"/>
+      <c r="D1" s="91"/>
+      <c r="E1" s="91"/>
+      <c r="F1" s="91"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="91"/>
+      <c r="I1" s="91"/>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
     </row>
     <row r="2" spans="1:11" ht="24" customHeight="1">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="98"/>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="98"/>
-      <c r="I2" s="98"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="92"/>
+      <c r="F2" s="92"/>
+      <c r="G2" s="92"/>
+      <c r="H2" s="92"/>
+      <c r="I2" s="92"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A3" s="99" t="s">
+      <c r="A3" s="93" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="99"/>
-      <c r="C3" s="99"/>
-      <c r="D3" s="99"/>
-      <c r="E3" s="99"/>
-      <c r="F3" s="99"/>
-      <c r="G3" s="99"/>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
+      <c r="B3" s="93"/>
+      <c r="C3" s="93"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+      <c r="I3" s="93"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A4" s="104" t="s">
+      <c r="A4" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="104"/>
-      <c r="C4" s="104"/>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="104"/>
-      <c r="H4" s="104"/>
-      <c r="I4" s="104"/>
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="G4" s="102"/>
+      <c r="H4" s="102"/>
+      <c r="I4" s="102"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
     <row r="5" spans="1:11" ht="21.95" customHeight="1">
-      <c r="A5" s="100" t="s">
+      <c r="A5" s="94" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="100"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="100"/>
-      <c r="I5" s="100"/>
+      <c r="B5" s="94"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
       <c r="J5" s="28"/>
       <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="54" customHeight="1">
-      <c r="A6" s="92" t="s">
+      <c r="A6" s="96" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="92"/>
-      <c r="C6" s="92"/>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="92"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+      <c r="I6" s="96"/>
       <c r="J6" s="33"/>
       <c r="K6" s="33"/>
     </row>
@@ -3292,12 +4533,12 @@
     </row>
     <row r="14" spans="1:11" ht="25.5" customHeight="1">
       <c r="A14" s="12"/>
-      <c r="B14" s="103" t="s">
+      <c r="B14" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="103"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="103"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="101"/>
+      <c r="E14" s="101"/>
       <c r="F14" s="17"/>
       <c r="G14" s="4"/>
       <c r="I14" s="3"/>
@@ -3390,14 +4631,14 @@
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="36"/>
-      <c r="L22" s="101"/>
+      <c r="L22" s="103"/>
     </row>
     <row r="23" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A23" s="94" t="s">
+      <c r="A23" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="94"/>
-      <c r="C23" s="94"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="98"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="6"/>
@@ -3406,16 +4647,16 @@
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="101"/>
+      <c r="L23" s="103"/>
     </row>
     <row r="24" spans="1:12" ht="72" customHeight="1">
       <c r="A24" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="95" t="s">
+      <c r="B24" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="95"/>
+      <c r="C24" s="99"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
@@ -3427,11 +4668,11 @@
       <c r="L24" s="29"/>
     </row>
     <row r="25" spans="1:12" ht="48" customHeight="1">
-      <c r="A25" s="96" t="s">
+      <c r="A25" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="96"/>
-      <c r="C25" s="96"/>
+      <c r="B25" s="100"/>
+      <c r="C25" s="100"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
@@ -3443,34 +4684,34 @@
       <c r="L25" s="29"/>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
-      <c r="A26" s="91" t="s">
+      <c r="A26" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="91"/>
-      <c r="F26" s="91"/>
-      <c r="G26" s="91"/>
-      <c r="H26" s="91"/>
-      <c r="I26" s="91"/>
-      <c r="J26" s="91"/>
-      <c r="K26" s="91"/>
+      <c r="B26" s="95"/>
+      <c r="C26" s="95"/>
+      <c r="D26" s="95"/>
+      <c r="E26" s="95"/>
+      <c r="F26" s="95"/>
+      <c r="G26" s="95"/>
+      <c r="H26" s="95"/>
+      <c r="I26" s="95"/>
+      <c r="J26" s="95"/>
+      <c r="K26" s="95"/>
     </row>
     <row r="27" spans="1:12" s="2" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A27" s="91" t="s">
+      <c r="A27" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="91"/>
-      <c r="C27" s="91"/>
-      <c r="D27" s="91"/>
-      <c r="E27" s="91"/>
-      <c r="F27" s="91"/>
-      <c r="G27" s="91"/>
-      <c r="H27" s="91"/>
-      <c r="I27" s="91"/>
-      <c r="J27" s="91"/>
-      <c r="K27" s="91"/>
+      <c r="B27" s="95"/>
+      <c r="C27" s="95"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="95"/>
+      <c r="F27" s="95"/>
+      <c r="G27" s="95"/>
+      <c r="H27" s="95"/>
+      <c r="I27" s="95"/>
+      <c r="J27" s="95"/>
+      <c r="K27" s="95"/>
     </row>
     <row r="28" spans="1:12" ht="27" customHeight="1">
       <c r="F28" s="6"/>
@@ -3494,8 +4735,8 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
-      <c r="J31" s="102"/>
-      <c r="K31" s="102"/>
+      <c r="J31" s="104"/>
+      <c r="K31" s="104"/>
     </row>
     <row r="32" spans="1:12" ht="53.1" customHeight="1">
       <c r="F32" s="6"/>
@@ -3526,6 +4767,13 @@
     <row r="63" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:K26"/>
+    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="J31:K31"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="B24:C24"/>
     <mergeCell ref="A6:I6"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="A1:I1"/>
@@ -3533,13 +4781,6 @@
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A4:I4"/>
     <mergeCell ref="A5:I5"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A27:K27"/>
-    <mergeCell ref="J31:K31"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="B24:C24"/>
   </mergeCells>
   <conditionalFormatting sqref="N23:N35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -3551,6 +4792,5 @@
   <rowBreaks count="1" manualBreakCount="1">
     <brk id="43" max="16383" man="1"/>
   </rowBreaks>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding fob fallback on desc
</commit_message>
<xml_diff>
--- a/TEMPLATE/MOTO.xlsx
+++ b/TEMPLATE/MOTO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JPZ031127\Desktop\refactor code\TEMPLATE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8A1599-A192-4780-A26A-D7322EA68FA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4208FDB2-9D1C-4E8B-A909-29737B942067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Contract" sheetId="1" r:id="rId1"/>
@@ -909,6 +909,24 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -921,34 +939,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -1234,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFD79"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:G29"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="85" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="15"/>
@@ -3913,8 +3913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -3933,70 +3933,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="38.25" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
     </row>
     <row r="2" spans="1:7" ht="24" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
     </row>
     <row r="3" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="99" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="93"/>
-      <c r="C4" s="93"/>
-      <c r="D4" s="93"/>
-      <c r="E4" s="93"/>
-      <c r="F4" s="93"/>
-      <c r="G4" s="93"/>
+      <c r="B4" s="99"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="99"/>
+      <c r="E4" s="99"/>
+      <c r="F4" s="99"/>
+      <c r="G4" s="99"/>
     </row>
     <row r="5" spans="1:7" ht="25.5" customHeight="1">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
     </row>
     <row r="6" spans="1:7" ht="69" customHeight="1">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="6"/>
@@ -4099,12 +4099,12 @@
     </row>
     <row r="15" spans="1:7" ht="25.5" customHeight="1">
       <c r="A15" s="35"/>
-      <c r="B15" s="97" t="s">
+      <c r="B15" s="93" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="97"/>
-      <c r="D15" s="97"/>
-      <c r="E15" s="97"/>
+      <c r="C15" s="93"/>
+      <c r="D15" s="93"/>
+      <c r="E15" s="93"/>
       <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:7" ht="25.5" customHeight="1">
@@ -4172,11 +4172,11 @@
       <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:7" ht="42" customHeight="1">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
       <c r="D23" s="24"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
@@ -4186,47 +4186,47 @@
       <c r="A24" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="99" t="s">
+      <c r="B24" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="99"/>
+      <c r="C24" s="95"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="6"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="44.1" customHeight="1">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="96" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="100"/>
-      <c r="C25" s="100"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" ht="24.75" customHeight="1">
-      <c r="A26" s="95" t="s">
+      <c r="A26" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="95"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
     </row>
     <row r="27" spans="1:7" s="2" customFormat="1" ht="27" customHeight="1">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
     </row>
     <row r="28" spans="1:7" ht="42" customHeight="1">
       <c r="E28" s="35"/>
@@ -4278,6 +4278,11 @@
     <row r="63" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A4:G4"/>
+    <mergeCell ref="A5:G5"/>
     <mergeCell ref="A26:G26"/>
     <mergeCell ref="A27:G27"/>
     <mergeCell ref="A6:G6"/>
@@ -4285,11 +4290,6 @@
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A4:G4"/>
-    <mergeCell ref="A5:G5"/>
   </mergeCells>
   <conditionalFormatting sqref="J23:J35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>
@@ -4305,8 +4305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L63"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A19" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28:L30"/>
+    <sheetView view="pageBreakPreview" topLeftCell="A7" zoomScale="85" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="15"/>
@@ -4314,7 +4314,7 @@
     <col min="1" max="1" width="29.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="25.85546875" style="3" customWidth="1"/>
     <col min="3" max="3" width="23.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="3" customWidth="1"/>
     <col min="5" max="5" width="21.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" style="3" customWidth="1"/>
@@ -4331,92 +4331,92 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="38.25" customHeight="1">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="97" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="91"/>
-      <c r="G1" s="91"/>
-      <c r="H1" s="91"/>
-      <c r="I1" s="91"/>
+      <c r="B1" s="97"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
       <c r="J1" s="32"/>
       <c r="K1" s="32"/>
     </row>
     <row r="2" spans="1:11" ht="24" customHeight="1">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="98" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
-      <c r="D2" s="92"/>
-      <c r="E2" s="92"/>
-      <c r="F2" s="92"/>
-      <c r="G2" s="92"/>
-      <c r="H2" s="92"/>
-      <c r="I2" s="92"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="98"/>
+      <c r="I2" s="98"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A3" s="93" t="s">
+      <c r="A3" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="93"/>
-      <c r="C3" s="93"/>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="93"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="99"/>
+      <c r="D3" s="99"/>
+      <c r="E3" s="99"/>
+      <c r="F3" s="99"/>
+      <c r="G3" s="99"/>
+      <c r="H3" s="99"/>
+      <c r="I3" s="99"/>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
     </row>
     <row r="4" spans="1:11" ht="25.5" customHeight="1">
-      <c r="A4" s="102" t="s">
+      <c r="A4" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="102"/>
-      <c r="C4" s="102"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="102"/>
-      <c r="F4" s="102"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="102"/>
-      <c r="I4" s="102"/>
+      <c r="B4" s="104"/>
+      <c r="C4" s="104"/>
+      <c r="D4" s="104"/>
+      <c r="E4" s="104"/>
+      <c r="F4" s="104"/>
+      <c r="G4" s="104"/>
+      <c r="H4" s="104"/>
+      <c r="I4" s="104"/>
       <c r="J4" s="28"/>
       <c r="K4" s="28"/>
     </row>
     <row r="5" spans="1:11" ht="21.95" customHeight="1">
-      <c r="A5" s="94" t="s">
+      <c r="A5" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="94"/>
-      <c r="C5" s="94"/>
-      <c r="D5" s="94"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
-      <c r="H5" s="94"/>
-      <c r="I5" s="94"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
       <c r="J5" s="28"/>
       <c r="K5" s="28"/>
     </row>
     <row r="6" spans="1:11" ht="54" customHeight="1">
-      <c r="A6" s="96" t="s">
+      <c r="A6" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="92"/>
       <c r="J6" s="33"/>
       <c r="K6" s="33"/>
     </row>
@@ -4533,12 +4533,12 @@
     </row>
     <row r="14" spans="1:11" ht="25.5" customHeight="1">
       <c r="A14" s="12"/>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="103" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="101"/>
-      <c r="D14" s="101"/>
-      <c r="E14" s="101"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
       <c r="F14" s="17"/>
       <c r="G14" s="4"/>
       <c r="I14" s="3"/>
@@ -4631,14 +4631,14 @@
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
       <c r="I22" s="36"/>
-      <c r="L22" s="103"/>
+      <c r="L22" s="101"/>
     </row>
     <row r="23" spans="1:12" ht="35.1" customHeight="1">
-      <c r="A23" s="98" t="s">
+      <c r="A23" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="B23" s="98"/>
-      <c r="C23" s="98"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="94"/>
       <c r="D23" s="24"/>
       <c r="E23" s="24"/>
       <c r="F23" s="6"/>
@@ -4647,16 +4647,16 @@
       <c r="I23" s="5"/>
       <c r="J23" s="6"/>
       <c r="K23" s="6"/>
-      <c r="L23" s="103"/>
+      <c r="L23" s="101"/>
     </row>
     <row r="24" spans="1:12" ht="72" customHeight="1">
       <c r="A24" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="99" t="s">
+      <c r="B24" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="99"/>
+      <c r="C24" s="95"/>
       <c r="D24" s="26"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
@@ -4668,11 +4668,11 @@
       <c r="L24" s="29"/>
     </row>
     <row r="25" spans="1:12" ht="48" customHeight="1">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="96" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="100"/>
-      <c r="C25" s="100"/>
+      <c r="B25" s="96"/>
+      <c r="C25" s="96"/>
       <c r="D25" s="27"/>
       <c r="E25" s="27"/>
       <c r="F25" s="27"/>
@@ -4684,34 +4684,34 @@
       <c r="L25" s="29"/>
     </row>
     <row r="26" spans="1:12" ht="30" customHeight="1">
-      <c r="A26" s="95" t="s">
+      <c r="A26" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="95"/>
-      <c r="C26" s="95"/>
-      <c r="D26" s="95"/>
-      <c r="E26" s="95"/>
-      <c r="F26" s="95"/>
-      <c r="G26" s="95"/>
-      <c r="H26" s="95"/>
-      <c r="I26" s="95"/>
-      <c r="J26" s="95"/>
-      <c r="K26" s="95"/>
+      <c r="B26" s="91"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="91"/>
+      <c r="E26" s="91"/>
+      <c r="F26" s="91"/>
+      <c r="G26" s="91"/>
+      <c r="H26" s="91"/>
+      <c r="I26" s="91"/>
+      <c r="J26" s="91"/>
+      <c r="K26" s="91"/>
     </row>
     <row r="27" spans="1:12" s="2" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A27" s="95" t="s">
+      <c r="A27" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="95"/>
-      <c r="C27" s="95"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="95"/>
-      <c r="F27" s="95"/>
-      <c r="G27" s="95"/>
-      <c r="H27" s="95"/>
-      <c r="I27" s="95"/>
-      <c r="J27" s="95"/>
-      <c r="K27" s="95"/>
+      <c r="B27" s="91"/>
+      <c r="C27" s="91"/>
+      <c r="D27" s="91"/>
+      <c r="E27" s="91"/>
+      <c r="F27" s="91"/>
+      <c r="G27" s="91"/>
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="91"/>
     </row>
     <row r="28" spans="1:12" ht="27" customHeight="1">
       <c r="F28" s="6"/>
@@ -4735,8 +4735,8 @@
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
-      <c r="J31" s="104"/>
-      <c r="K31" s="104"/>
+      <c r="J31" s="102"/>
+      <c r="K31" s="102"/>
     </row>
     <row r="32" spans="1:12" ht="53.1" customHeight="1">
       <c r="F32" s="6"/>
@@ -4767,6 +4767,13 @@
     <row r="63" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:I6"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="A3:I3"/>
+    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A5:I5"/>
     <mergeCell ref="L22:L23"/>
     <mergeCell ref="A25:C25"/>
     <mergeCell ref="A26:K26"/>
@@ -4774,13 +4781,6 @@
     <mergeCell ref="J31:K31"/>
     <mergeCell ref="A23:C23"/>
     <mergeCell ref="B24:C24"/>
-    <mergeCell ref="A6:I6"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A3:I3"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="A5:I5"/>
   </mergeCells>
   <conditionalFormatting sqref="N23:N35">
     <cfRule type="duplicateValues" priority="1" stopIfTrue="1"/>

</xml_diff>